<commit_message>
Added new and changes fiels
</commit_message>
<xml_diff>
--- a/TestData/Logins.xlsx
+++ b/TestData/Logins.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="1" windowHeight="8310" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="8310" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="valid" r:id="rId1" sheetId="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="420">
   <si>
     <t>username</t>
   </si>
@@ -1279,6 +1279,21 @@
   </si>
   <si>
     <t>access to view upp payment details</t>
+  </si>
+  <si>
+    <t>upptesting@unicity.com</t>
+  </si>
+  <si>
+    <t>upp@123</t>
+  </si>
+  <si>
+    <t>Upp user</t>
+  </si>
+  <si>
+    <t>Deepa M</t>
+  </si>
+  <si>
+    <t>Ranjith</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1387,30 +1402,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1423,7 +1414,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
@@ -1471,8 +1462,6 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
     <xf applyBorder="1" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="1">
       <alignment horizontal="left"/>
@@ -1480,15 +1469,15 @@
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="5" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="3" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1771,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,7 +1856,7 @@
       <c r="E5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="25" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1915,7 +1904,7 @@
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="23" t="s">
@@ -1923,20 +1912,31 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="2" t="s">
         <v>302</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -1959,9 +1959,11 @@
     <hyperlink r:id="rId16" ref="E9"/>
     <hyperlink r:id="rId17" ref="E8"/>
     <hyperlink r:id="rId18" ref="F5"/>
+    <hyperlink r:id="rId19" ref="A10"/>
+    <hyperlink r:id="rId20" ref="B10"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -1981,11 +1983,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -2024,11 +2026,11 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>330</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -2062,11 +2064,11 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>334</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
@@ -2106,11 +2108,11 @@
       <c r="C16" s="17"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>336</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -2154,11 +2156,11 @@
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
@@ -2201,11 +2203,11 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="31" t="s">
         <v>344</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
@@ -2239,11 +2241,11 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
@@ -2277,11 +2279,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="31" t="s">
         <v>346</v>
       </c>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
@@ -2322,11 +2324,11 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="31" t="s">
         <v>347</v>
       </c>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
@@ -2343,7 +2345,7 @@
       <c r="A50" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="26" t="s">
         <v>357</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -2413,11 +2415,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>336</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -2454,11 +2456,11 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>330</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -2488,11 +2490,11 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
@@ -2538,15 +2540,15 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="C17" s="30"/>
+      <c r="A17" s="29"/>
+      <c r="C17" s="28"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>371</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -2601,11 +2603,11 @@
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="31" t="s">
         <v>346</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
@@ -2646,11 +2648,11 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>347</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
@@ -2667,7 +2669,7 @@
       <c r="A34" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="26" t="s">
         <v>357</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -2701,11 +2703,11 @@
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="31" t="s">
         <v>382</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
@@ -2719,7 +2721,7 @@
       </c>
     </row>
     <row ht="30" r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="27" t="s">
         <v>391</v>
       </c>
       <c r="B41" s="19" t="s">
@@ -3773,7 +3775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
@@ -4470,7 +4472,7 @@
       <c r="A63" s="8">
         <v>63</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C63" s="9" t="s">
@@ -4481,10 +4483,10 @@
       <c r="A64" s="8">
         <v>64</v>
       </c>
-      <c r="B64" s="33" t="s">
+      <c r="B64" s="30" t="s">
         <v>395</v>
       </c>
-      <c r="C64" s="33" t="s">
+      <c r="C64" s="30" t="s">
         <v>396</v>
       </c>
     </row>
@@ -4492,10 +4494,10 @@
       <c r="A65" s="8">
         <v>65</v>
       </c>
-      <c r="B65" s="33" t="s">
+      <c r="B65" s="30" t="s">
         <v>397</v>
       </c>
-      <c r="C65" s="33" t="s">
+      <c r="C65" s="30" t="s">
         <v>398</v>
       </c>
     </row>
@@ -4506,7 +4508,7 @@
       <c r="B66" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="C66" s="33" t="s">
+      <c r="C66" s="30" t="s">
         <v>400</v>
       </c>
     </row>
@@ -4514,10 +4516,10 @@
       <c r="A67" s="8">
         <v>67</v>
       </c>
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="30" t="s">
         <v>401</v>
       </c>
-      <c r="C67" s="33" t="s">
+      <c r="C67" s="30" t="s">
         <v>402</v>
       </c>
     </row>
@@ -4525,10 +4527,10 @@
       <c r="A68" s="8">
         <v>68</v>
       </c>
-      <c r="B68" s="33" t="s">
+      <c r="B68" s="30" t="s">
         <v>403</v>
       </c>
-      <c r="C68" s="33" t="s">
+      <c r="C68" s="30" t="s">
         <v>400</v>
       </c>
     </row>
@@ -4536,10 +4538,10 @@
       <c r="A69" s="8">
         <v>69</v>
       </c>
-      <c r="B69" s="33" t="s">
+      <c r="B69" s="30" t="s">
         <v>404</v>
       </c>
-      <c r="C69" s="33" t="s">
+      <c r="C69" s="30" t="s">
         <v>405</v>
       </c>
     </row>
@@ -4547,10 +4549,10 @@
       <c r="A70" s="8">
         <v>70</v>
       </c>
-      <c r="B70" s="33" t="s">
+      <c r="B70" s="30" t="s">
         <v>406</v>
       </c>
-      <c r="C70" s="33" t="s">
+      <c r="C70" s="30" t="s">
         <v>407</v>
       </c>
     </row>
@@ -4558,10 +4560,10 @@
       <c r="A71" s="8">
         <v>71</v>
       </c>
-      <c r="B71" s="33" t="s">
+      <c r="B71" s="30" t="s">
         <v>408</v>
       </c>
-      <c r="C71" s="33" t="s">
+      <c r="C71" s="30" t="s">
         <v>409</v>
       </c>
     </row>
@@ -4569,10 +4571,10 @@
       <c r="A72" s="8">
         <v>72</v>
       </c>
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="30" t="s">
         <v>410</v>
       </c>
-      <c r="C72" s="33" t="s">
+      <c r="C72" s="30" t="s">
         <v>411</v>
       </c>
     </row>
@@ -4580,10 +4582,10 @@
       <c r="A73" s="8">
         <v>73</v>
       </c>
-      <c r="B73" s="33" t="s">
+      <c r="B73" s="30" t="s">
         <v>412</v>
       </c>
-      <c r="C73" s="33" t="s">
+      <c r="C73" s="30" t="s">
         <v>411</v>
       </c>
     </row>
@@ -4591,10 +4593,10 @@
       <c r="A74" s="8">
         <v>74</v>
       </c>
-      <c r="B74" s="33" t="s">
+      <c r="B74" s="30" t="s">
         <v>413</v>
       </c>
-      <c r="C74" s="33" t="s">
+      <c r="C74" s="30" t="s">
         <v>414</v>
       </c>
     </row>
@@ -5048,11 +5050,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -5109,11 +5111,11 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
@@ -5147,11 +5149,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -5197,11 +5199,11 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -5247,11 +5249,11 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
@@ -5287,11 +5289,11 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
@@ -5327,11 +5329,11 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
@@ -5365,11 +5367,11 @@
       <c r="C41" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
@@ -5405,11 +5407,11 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
@@ -5445,11 +5447,11 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="32" t="s">
+      <c r="A56" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
@@ -5492,11 +5494,11 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="32" t="s">
+      <c r="A63" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="31"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
@@ -5532,11 +5534,11 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="32" t="s">
+      <c r="A69" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="32"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="31"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
@@ -5561,11 +5563,11 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="32" t="s">
+      <c r="A74" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32"/>
+      <c r="B74" s="31"/>
+      <c r="C74" s="31"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
@@ -5599,11 +5601,11 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="32" t="s">
+      <c r="A79" s="31" t="s">
         <v>269</v>
       </c>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32"/>
+      <c r="B79" s="31"/>
+      <c r="C79" s="31"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
@@ -5638,11 +5640,11 @@
       <c r="C83" s="21"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="32" t="s">
+      <c r="A84" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="B84" s="32"/>
-      <c r="C84" s="32"/>
+      <c r="B84" s="31"/>
+      <c r="C84" s="31"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
@@ -5674,11 +5676,11 @@
       <c r="C87" s="18"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="32" t="s">
+      <c r="A90" s="31" t="s">
         <v>274</v>
       </c>
-      <c r="B90" s="32"/>
-      <c r="C90" s="32"/>
+      <c r="B90" s="31"/>
+      <c r="C90" s="31"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
@@ -5710,11 +5712,11 @@
       <c r="C93" s="18"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="32" t="s">
+      <c r="A96" s="31" t="s">
         <v>296</v>
       </c>
-      <c r="B96" s="32"/>
-      <c r="C96" s="32"/>
+      <c r="B96" s="31"/>
+      <c r="C96" s="31"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
@@ -5746,11 +5748,11 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="32" t="s">
+      <c r="A102" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="B102" s="32"/>
-      <c r="C102" s="32"/>
+      <c r="B102" s="31"/>
+      <c r="C102" s="31"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
@@ -5782,11 +5784,11 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="32" t="s">
+      <c r="A108" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="B108" s="32"/>
-      <c r="C108" s="32"/>
+      <c r="B108" s="31"/>
+      <c r="C108" s="31"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
@@ -5824,6 +5826,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A96:C96"/>
+    <mergeCell ref="A102:C102"/>
+    <mergeCell ref="A108:C108"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A90:C90"/>
     <mergeCell ref="A74:C74"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A8:C8"/>
@@ -5837,12 +5845,6 @@
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A96:C96"/>
-    <mergeCell ref="A102:C102"/>
-    <mergeCell ref="A108:C108"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A90:C90"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added other WH users scenarios
</commit_message>
<xml_diff>
--- a/TestData/Logins.xlsx
+++ b/TestData/Logins.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="8310" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="5" windowHeight="8310" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="valid" r:id="rId1" sheetId="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="412">
   <si>
     <t>username</t>
   </si>
@@ -984,36 +984,6 @@
     <t>RTO</t>
   </si>
   <si>
-    <t>Kyc</t>
-  </si>
-  <si>
-    <t>Users</t>
-  </si>
-  <si>
-    <t>Roles</t>
-  </si>
-  <si>
-    <t>Permissions</t>
-  </si>
-  <si>
-    <t>Warehouses</t>
-  </si>
-  <si>
-    <t>Countries</t>
-  </si>
-  <si>
-    <t>SMS Templates</t>
-  </si>
-  <si>
-    <t>UPP Payments</t>
-  </si>
-  <si>
-    <t>UPP Distributors</t>
-  </si>
-  <si>
-    <t>Send SMS</t>
-  </si>
-  <si>
     <t>UPP Distributor Name</t>
   </si>
   <si>
@@ -1290,10 +1260,16 @@
     <t>Upp user</t>
   </si>
   <si>
-    <t>Deepa M</t>
+    <t>Raipur WH</t>
   </si>
   <si>
     <t>Ranjith</t>
+  </si>
+  <si>
+    <t>Raipur</t>
+  </si>
+  <si>
+    <t>Dilip</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1409,12 +1385,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
@@ -1476,6 +1465,7 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf applyBorder="1" borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -1760,10 +1750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1783,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="31" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1813,7 +1803,7 @@
       <c r="A3" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1827,7 +1817,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1930,13 +1920,24 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>417</v>
+        <v>407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -1961,9 +1962,10 @@
     <hyperlink r:id="rId18" ref="F5"/>
     <hyperlink r:id="rId19" ref="A10"/>
     <hyperlink r:id="rId20" ref="B10"/>
+    <hyperlink r:id="rId21" ref="A11"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -1983,11 +1985,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>326</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="A1" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -2008,16 +2010,16 @@
         <v>249</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="1" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,11 +2028,11 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>330</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="A6" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -2048,27 +2050,27 @@
         <v>217</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="15" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>334</v>
-      </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
+      <c r="A11" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
@@ -2087,7 +2089,7 @@
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2108,11 +2110,11 @@
       <c r="C16" s="17"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
+      <c r="A18" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -2130,19 +2132,19 @@
         <v>217</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2156,11 +2158,11 @@
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
-        <v>339</v>
-      </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
+      <c r="A24" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
@@ -2178,10 +2180,10 @@
         <v>230</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2192,22 +2194,22 @@
         <v>213</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="17" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
-        <v>344</v>
-      </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
+      <c r="A30" s="32" t="s">
+        <v>334</v>
+      </c>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
@@ -2228,24 +2230,24 @@
         <v>172</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="1" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>345</v>
-      </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
+      <c r="A36" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
@@ -2263,27 +2265,27 @@
         <v>217</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="1" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
-        <v>346</v>
-      </c>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
+      <c r="A42" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
@@ -2298,37 +2300,37 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>261</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B45" s="15"/>
       <c r="C45" s="1" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="17" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="31" t="s">
-        <v>347</v>
-      </c>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
+      <c r="A48" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
@@ -2346,33 +2348,33 @@
         <v>228</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="18" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2415,11 +2417,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="A1" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -2438,16 +2440,16 @@
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="1" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2456,11 +2458,11 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>330</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="A6" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -2479,22 +2481,22 @@
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="1" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="15"/>
       <c r="C9" s="1" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>339</v>
-      </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
+      <c r="A11" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
@@ -2513,7 +2515,7 @@
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="1" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2522,21 +2524,21 @@
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="1" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="1"/>
       <c r="C15" s="17" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="1"/>
       <c r="C16" s="17" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2544,11 +2546,11 @@
       <c r="C17" s="28"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>371</v>
-      </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
+      <c r="A18" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -2566,35 +2568,35 @@
         <v>217</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="17" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="1"/>
       <c r="C23" s="17" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2603,11 +2605,11 @@
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
-        <v>346</v>
-      </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
+      <c r="A25" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
@@ -2622,37 +2624,37 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>261</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="1" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="17" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
-        <v>347</v>
-      </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
+      <c r="A32" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
@@ -2670,24 +2672,24 @@
         <v>228</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B35" s="15"/>
       <c r="C35" s="18" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2703,11 +2705,11 @@
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
-        <v>382</v>
-      </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
+      <c r="A39" s="32" t="s">
+        <v>372</v>
+      </c>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
@@ -2722,30 +2724,30 @@
     </row>
     <row ht="30" r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="C42" s="18"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C43" s="1"/>
     </row>
@@ -2883,47 +2885,47 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>316</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>317</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>318</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>319</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>322</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>323</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>324</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
@@ -2933,7 +2935,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
@@ -2948,22 +2950,22 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>325</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>304</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>305</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20">
@@ -3596,152 +3598,152 @@
         <v>28</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>28</v>
       </c>
@@ -4473,10 +4475,10 @@
         <v>63</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -4484,10 +4486,10 @@
         <v>64</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="C64" s="30" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -4495,10 +4497,10 @@
         <v>65</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -4506,10 +4508,10 @@
         <v>66</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="C66" s="30" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -4517,10 +4519,10 @@
         <v>67</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C67" s="30" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -4528,10 +4530,10 @@
         <v>68</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="C68" s="30" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -4539,10 +4541,10 @@
         <v>69</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C69" s="30" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -4550,10 +4552,10 @@
         <v>70</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="C70" s="30" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -4561,10 +4563,10 @@
         <v>71</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="C71" s="30" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -4572,10 +4574,10 @@
         <v>72</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="C72" s="30" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -4583,10 +4585,10 @@
         <v>73</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="C73" s="30" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -4594,10 +4596,10 @@
         <v>74</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="C74" s="30" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -4672,7 +4674,7 @@
         <v>301</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -4683,10 +4685,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4785,6 +4787,17 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>6</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -5050,11 +5063,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -5111,11 +5124,11 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
@@ -5149,11 +5162,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -5199,11 +5212,11 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="32" t="s">
         <v>226</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -5249,11 +5262,11 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
@@ -5289,11 +5302,11 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
@@ -5329,11 +5342,11 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
@@ -5367,11 +5380,11 @@
       <c r="C41" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
@@ -5407,11 +5420,11 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
@@ -5447,11 +5460,11 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
@@ -5494,11 +5507,11 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="31" t="s">
+      <c r="A63" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
@@ -5534,11 +5547,11 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="31" t="s">
+      <c r="A69" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="B69" s="31"/>
-      <c r="C69" s="31"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
@@ -5563,11 +5576,11 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="31" t="s">
+      <c r="A74" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="B74" s="31"/>
-      <c r="C74" s="31"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
@@ -5601,11 +5614,11 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="31" t="s">
+      <c r="A79" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="B79" s="31"/>
-      <c r="C79" s="31"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
@@ -5640,11 +5653,11 @@
       <c r="C83" s="21"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="31" t="s">
+      <c r="A84" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="B84" s="31"/>
-      <c r="C84" s="31"/>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
@@ -5676,11 +5689,11 @@
       <c r="C87" s="18"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="31" t="s">
+      <c r="A90" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="B90" s="31"/>
-      <c r="C90" s="31"/>
+      <c r="B90" s="32"/>
+      <c r="C90" s="32"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
@@ -5712,11 +5725,11 @@
       <c r="C93" s="18"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="31" t="s">
+      <c r="A96" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="B96" s="31"/>
-      <c r="C96" s="31"/>
+      <c r="B96" s="32"/>
+      <c r="C96" s="32"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
@@ -5748,11 +5761,11 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="31" t="s">
+      <c r="A102" s="32" t="s">
         <v>280</v>
       </c>
-      <c r="B102" s="31"/>
-      <c r="C102" s="31"/>
+      <c r="B102" s="32"/>
+      <c r="C102" s="32"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
@@ -5784,11 +5797,11 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="31" t="s">
+      <c r="A108" s="32" t="s">
         <v>286</v>
       </c>
-      <c r="B108" s="31"/>
-      <c r="C108" s="31"/>
+      <c r="B108" s="32"/>
+      <c r="C108" s="32"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">

</xml_diff>

<commit_message>
Modified login excel file
</commit_message>
<xml_diff>
--- a/TestData/Logins.xlsx
+++ b/TestData/Logins.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="423">
   <si>
     <t>username</t>
   </si>
@@ -1270,6 +1270,39 @@
   </si>
   <si>
     <t>Dilip</t>
+  </si>
+  <si>
+    <t>Kyc</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Permissions</t>
+  </si>
+  <si>
+    <t>Warehouses</t>
+  </si>
+  <si>
+    <t>Countries</t>
+  </si>
+  <si>
+    <t>SMS Templates</t>
+  </si>
+  <si>
+    <t>UPP Payments</t>
+  </si>
+  <si>
+    <t>UPP Distributors</t>
+  </si>
+  <si>
+    <t>Send SMS</t>
+  </si>
+  <si>
+    <t>Deepa M</t>
   </si>
 </sst>
 </file>
@@ -2885,12 +2918,12 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5">
@@ -2900,17 +2933,17 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>304</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>305</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -3598,152 +3631,152 @@
         <v>28</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146">
       <c r="A146" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147">
       <c r="A147" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148">
       <c r="A148" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149">
       <c r="A149" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150">
       <c r="A150" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151">
       <c r="A151" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152">
       <c r="A152" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153">
       <c r="A153" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154">
       <c r="A154" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155">
       <c r="A155" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156">
       <c r="A156" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157">
       <c r="A157" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158">
       <c r="A158" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159">
       <c r="A159" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160">
       <c r="A160" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161">
       <c r="A161" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162">
       <c r="A162" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163">
       <c r="A163" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164">
       <c r="A164" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165">
       <c r="A165" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166">
       <c r="A166" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167">
       <c r="A167" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168">
       <c r="A168" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169">
       <c r="A169" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170">
       <c r="A170" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171">
       <c r="A171" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172">
       <c r="A172" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173">
       <c r="A173" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174">
       <c r="A174" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175">
       <c r="A175" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
fixed couple of issues
</commit_message>
<xml_diff>
--- a/TestData/Logins.xlsx
+++ b/TestData/Logins.xlsx
@@ -1,32 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2-TestingProjects\Automation\Selenium\Warehouse\WHKYC\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="5" windowHeight="8310" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310"/>
   </bookViews>
   <sheets>
-    <sheet name="valid" r:id="rId1" sheetId="1"/>
-    <sheet name="Invalid" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet2" r:id="rId3" sheetId="4"/>
-    <sheet name="Permissions" r:id="rId4" sheetId="5"/>
-    <sheet name="Roles" r:id="rId5" sheetId="6"/>
-    <sheet name="Warehouses" r:id="rId6" sheetId="7"/>
-    <sheet name="Countries" r:id="rId7" sheetId="8"/>
-    <sheet name="SMSTemplates" r:id="rId8" sheetId="9"/>
-    <sheet name="CreateOrder" r:id="rId9" sheetId="10"/>
-    <sheet name="UppDistributorPage" r:id="rId10" sheetId="11"/>
-    <sheet name="UppPaymentPage" r:id="rId11" sheetId="12"/>
+    <sheet name="valid" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Permissions" sheetId="5" r:id="rId4"/>
+    <sheet name="Roles" sheetId="6" r:id="rId5"/>
+    <sheet name="Warehouses" sheetId="7" r:id="rId6"/>
+    <sheet name="Countries" sheetId="8" r:id="rId7"/>
+    <sheet name="SMSTemplates" sheetId="9" r:id="rId8"/>
+    <sheet name="CreateOrder" sheetId="10" r:id="rId9"/>
+    <sheet name="UppDistributorPage" sheetId="11" r:id="rId10"/>
+    <sheet name="UppPaymentPage" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="420">
   <si>
     <t>username</t>
   </si>
@@ -1263,13 +1263,7 @@
     <t>Raipur WH</t>
   </si>
   <si>
-    <t>Ranjith</t>
-  </si>
-  <si>
     <t>Raipur</t>
-  </si>
-  <si>
-    <t>Dilip</t>
   </si>
   <si>
     <t>Kyc</t>
@@ -1306,7 +1300,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1430,82 +1423,82 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="3" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1522,10 +1515,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1560,7 +1553,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1595,7 +1588,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1689,21 +1682,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1720,7 +1713,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1772,27 +1765,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1918,8 +1911,8 @@
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>20</v>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -1935,8 +1928,8 @@
       <c r="A9" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>303</v>
@@ -1972,36 +1965,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A4"/>
-    <hyperlink r:id="rId3" ref="A5"/>
-    <hyperlink r:id="rId4" ref="A6"/>
-    <hyperlink r:id="rId5" ref="A7"/>
-    <hyperlink r:id="rId6" ref="B7"/>
-    <hyperlink r:id="rId7" ref="A8"/>
-    <hyperlink r:id="rId8" ref="E2"/>
-    <hyperlink r:id="rId9" ref="F2"/>
-    <hyperlink display="mailto:Ashwin.GS@unicity.com" r:id="rId10" ref="A3"/>
-    <hyperlink r:id="rId11" ref="E7"/>
-    <hyperlink r:id="rId12" ref="F7"/>
-    <hyperlink r:id="rId13" ref="E3"/>
-    <hyperlink r:id="rId14" ref="F3"/>
-    <hyperlink display="mailto:DSCNEindia.unicity@outlook.com" r:id="rId15" ref="A9"/>
-    <hyperlink r:id="rId16" ref="E9"/>
-    <hyperlink r:id="rId17" ref="E8"/>
-    <hyperlink r:id="rId18" ref="F5"/>
-    <hyperlink r:id="rId19" ref="A10"/>
-    <hyperlink r:id="rId20" ref="B10"/>
-    <hyperlink r:id="rId21" ref="A11"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="E2" r:id="rId8"/>
+    <hyperlink ref="F2" r:id="rId9"/>
+    <hyperlink ref="A3" r:id="rId10" display="mailto:Ashwin.GS@unicity.com"/>
+    <hyperlink ref="E7" r:id="rId11"/>
+    <hyperlink ref="F7" r:id="rId12"/>
+    <hyperlink ref="E3" r:id="rId13"/>
+    <hyperlink ref="F3" r:id="rId14"/>
+    <hyperlink ref="A9" r:id="rId15" display="mailto:DSCNEindia.unicity@outlook.com"/>
+    <hyperlink ref="E9" r:id="rId16"/>
+    <hyperlink ref="E8" r:id="rId17"/>
+    <hyperlink ref="F5" r:id="rId18"/>
+    <hyperlink ref="A10" r:id="rId19"/>
+    <hyperlink ref="B10" r:id="rId20"/>
+    <hyperlink ref="A11" r:id="rId21"/>
+    <hyperlink ref="B8" r:id="rId22"/>
+    <hyperlink ref="B9" r:id="rId23"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
@@ -2009,9 +2004,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="74.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="74.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2422,18 +2417,18 @@
     <mergeCell ref="A30:C30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B50"/>
-    <hyperlink r:id="rId2" ref="A52"/>
-    <hyperlink r:id="rId3" ref="A53"/>
+    <hyperlink ref="B50" r:id="rId1"/>
+    <hyperlink ref="A52" r:id="rId2"/>
+    <hyperlink ref="A53" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
@@ -2441,9 +2436,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="74.140625" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="74.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2729,7 +2724,7 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row customHeight="1" ht="12.75" r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2752,7 +2747,7 @@
         <v>210</v>
       </c>
     </row>
-    <row ht="30" r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>381</v>
       </c>
@@ -2792,16 +2787,16 @@
     <mergeCell ref="A25:C25"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B34"/>
-    <hyperlink r:id="rId2" ref="A36"/>
+    <hyperlink ref="B34" r:id="rId1"/>
+    <hyperlink ref="A36" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
@@ -2809,10 +2804,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2877,25 +2872,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A4"/>
-    <hyperlink r:id="rId2" ref="A5"/>
-    <hyperlink r:id="rId3" ref="B5"/>
-    <hyperlink r:id="rId4" ref="A6"/>
-    <hyperlink display="mailto:jamalpur_acc@omlogistics.co.in" r:id="rId5" ref="A2"/>
-    <hyperlink r:id="rId6" ref="A3"/>
-    <hyperlink r:id="rId7" ref="B4"/>
-    <hyperlink r:id="rId8" ref="B6"/>
-    <hyperlink r:id="rId9" ref="D2"/>
-    <hyperlink r:id="rId10" ref="E2"/>
+    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId5" display="mailto:jamalpur_acc@omlogistics.co.in"/>
+    <hyperlink ref="A3" r:id="rId6"/>
+    <hyperlink ref="B4" r:id="rId7"/>
+    <hyperlink ref="B6" r:id="rId8"/>
+    <hyperlink ref="D2" r:id="rId9"/>
+    <hyperlink ref="E2" r:id="rId10"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B179"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
@@ -2903,877 +2898,877 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="12">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>28</v>
       </c>
@@ -3799,13 +3794,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
@@ -3813,9 +3808,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="7" width="30.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="7" width="53.28515625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="7" collapsed="1"/>
+    <col min="2" max="2" width="30.85546875" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="53.28515625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4633,14 +4628,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -4648,8 +4643,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="54" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4708,24 +4703,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="5.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4823,21 +4818,21 @@
         <v>6</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -4857,13 +4852,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
@@ -4871,8 +4866,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="137.0" collapsed="true"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="137" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4903,7 +4898,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="30" r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -4917,7 +4912,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="30" r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>4</v>
       </c>
@@ -4931,7 +4926,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="45" r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>5</v>
       </c>
@@ -4945,7 +4940,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="30" r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>6</v>
       </c>
@@ -4959,7 +4954,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="30" r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>7</v>
       </c>
@@ -4973,7 +4968,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="30" r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>8</v>
       </c>
@@ -4987,7 +4982,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="30" r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>9</v>
       </c>
@@ -5015,7 +5010,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="45" r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>11</v>
       </c>
@@ -5029,7 +5024,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="30" r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>12</v>
       </c>
@@ -5043,7 +5038,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="30" r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>13</v>
       </c>
@@ -5057,7 +5052,7 @@
         <v>175</v>
       </c>
     </row>
-    <row ht="30" r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>14</v>
       </c>
@@ -5072,14 +5067,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B52" sqref="B52:B53"/>
@@ -5087,9 +5082,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="74.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="74.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5478,7 +5473,7 @@
         <v>247</v>
       </c>
     </row>
-    <row ht="30" r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>252</v>
       </c>
@@ -5700,7 +5695,7 @@
         <v>210</v>
       </c>
     </row>
-    <row ht="30" r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
         <v>251</v>
       </c>
@@ -5781,7 +5776,7 @@
         <v>279</v>
       </c>
     </row>
-    <row ht="30" r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="19" t="s">
         <v>224</v>
       </c>
@@ -5869,12 +5864,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A96:C96"/>
-    <mergeCell ref="A102:C102"/>
-    <mergeCell ref="A108:C108"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A90:C90"/>
     <mergeCell ref="A74:C74"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A8:C8"/>
@@ -5888,8 +5877,14 @@
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A96:C96"/>
+    <mergeCell ref="A102:C102"/>
+    <mergeCell ref="A108:C108"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A90:C90"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added LIVE data check scenario
</commit_message>
<xml_diff>
--- a/TestData/Logins.xlsx
+++ b/TestData/Logins.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="415">
   <si>
     <t>username</t>
   </si>
@@ -426,75 +426,36 @@
     <t>kyc_store</t>
   </si>
   <si>
-    <t>User will be able to store the KYC details</t>
-  </si>
-  <si>
     <t>kyc_show</t>
   </si>
   <si>
-    <t>User will b able to view the KYC details</t>
-  </si>
-  <si>
     <t>kyc_edit</t>
   </si>
   <si>
-    <t>User will be able to view the validate page</t>
-  </si>
-  <si>
     <t>kyc_update@store</t>
   </si>
   <si>
-    <t>User will be able to store the kyc Validation changes</t>
-  </si>
-  <si>
-    <t>kyc_uploadexcel1</t>
-  </si>
-  <si>
-    <t>User will be able to upload the KYC excel sheet</t>
-  </si>
-  <si>
     <t>kyc_searchkyc@store</t>
   </si>
   <si>
-    <t>User should be able to search</t>
-  </si>
-  <si>
     <t>kyc_uploadexcel</t>
   </si>
   <si>
-    <t>Upload Excel sheet in to KYC portal</t>
-  </si>
-  <si>
     <t>kyc_zipdownload</t>
   </si>
   <si>
-    <t>access to download distributors uploaded kyc docs</t>
-  </si>
-  <si>
     <t>kyc_sendsms</t>
   </si>
   <si>
-    <t>sending sms in kyc page</t>
-  </si>
-  <si>
     <t>smstemplates_index</t>
   </si>
   <si>
-    <t>permission to create</t>
-  </si>
-  <si>
     <t>smstemplates_create</t>
   </si>
   <si>
-    <t>to create SMS permission</t>
-  </si>
-  <si>
     <t>smstemplates_store</t>
   </si>
   <si>
-    <t>Creating permision on save</t>
-  </si>
-  <si>
     <t>smstemplates_edit</t>
   </si>
   <si>
@@ -516,9 +477,6 @@
     <t>kyc_exportexcel</t>
   </si>
   <si>
-    <t>To export the excel file</t>
-  </si>
-  <si>
     <t>The Super admin of the system</t>
   </si>
   <si>
@@ -564,9 +522,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>Dear Unicity Distributor, Thank you for uploading all the necessary documents, please be informed that the ID number [DIST_ID] has been ACTIVATED.</t>
-  </si>
-  <si>
     <t>Pan Card Pending</t>
   </si>
   <si>
@@ -1173,9 +1128,6 @@
     <t>M/S New Look Unicity Testing</t>
   </si>
   <si>
-    <t>Assigned under this role can access only UPP related pages</t>
-  </si>
-  <si>
     <t>Global fortune Creators</t>
   </si>
   <si>
@@ -1197,15 +1149,6 @@
     <t>access to see listing of payments done by upp distributors</t>
   </si>
   <si>
-    <t>upppayments_create</t>
-  </si>
-  <si>
-    <t>To create upp payment</t>
-  </si>
-  <si>
-    <t>upppayments_store</t>
-  </si>
-  <si>
     <t>store the details in DB</t>
   </si>
   <si>
@@ -1245,12 +1188,6 @@
     <t>uppdistributors_show</t>
   </si>
   <si>
-    <t>upppayments_paymentresponse</t>
-  </si>
-  <si>
-    <t>access to view upp payment details</t>
-  </si>
-  <si>
     <t>upptesting@unicity.com</t>
   </si>
   <si>
@@ -1294,6 +1231,54 @@
   </si>
   <si>
     <t>Send SMS</t>
+  </si>
+  <si>
+    <t>User will be able to upload the kYC</t>
+  </si>
+  <si>
+    <t>User will be able to view the KYC of each ID in details</t>
+  </si>
+  <si>
+    <t>User will be able to view KYC validate page</t>
+  </si>
+  <si>
+    <t>User will be able to update the validation of the kyc</t>
+  </si>
+  <si>
+    <t>User will be able to search the KYC</t>
+  </si>
+  <si>
+    <t>User will be able to upload the KYC report excel</t>
+  </si>
+  <si>
+    <t>access to download kyc documents</t>
+  </si>
+  <si>
+    <t>User will be able to send SMS to the Distributor</t>
+  </si>
+  <si>
+    <t>User can able to see the sms templates listing</t>
+  </si>
+  <si>
+    <t>User can able to create sms templates</t>
+  </si>
+  <si>
+    <t>User can able to save created sms templates</t>
+  </si>
+  <si>
+    <t>User will be able to download the KYC report</t>
+  </si>
+  <si>
+    <t>access for upp payments and upp distributors modules</t>
+  </si>
+  <si>
+    <t>Testing SMS Template</t>
+  </si>
+  <si>
+    <t>Testing SMS template content</t>
+  </si>
+  <si>
+    <t>Dear Unicity Distributor, Thank you for uploading all the necessary documents, please be informed that the ID number [DIST_ID] has been ACTIVATED</t>
   </si>
 </sst>
 </file>
@@ -1426,7 +1411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1489,6 +1474,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1775,7 +1763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1824,7 +1812,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1926,13 +1914,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>20</v>
@@ -1943,24 +1931,24 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>406</v>
+        <v>385</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>407</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>408</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -2010,41 +1998,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="1" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2053,73 +2041,73 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>320</v>
-      </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
+      <c r="A6" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="15" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
-        <v>324</v>
-      </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="A11" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="1" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2135,41 +2123,41 @@
       <c r="C16" s="17"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
-        <v>326</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
+      <c r="A18" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2183,223 +2171,223 @@
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
-        <v>329</v>
-      </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
+      <c r="A24" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="17" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
-        <v>334</v>
-      </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
+      <c r="A30" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="1" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
-        <v>335</v>
-      </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
+      <c r="A36" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="1" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
-        <v>336</v>
-      </c>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
+      <c r="A42" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="B45" s="15"/>
       <c r="C45" s="1" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="17" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
+      <c r="A48" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="18" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2442,39 +2430,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>326</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="1" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2483,87 +2471,87 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>320</v>
-      </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
+      <c r="A6" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="1" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="15"/>
       <c r="C9" s="1" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
-        <v>329</v>
-      </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="A11" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="1" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="1" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="1"/>
       <c r="C15" s="17" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="1"/>
       <c r="C16" s="17" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2571,57 +2559,57 @@
       <c r="C17" s="28"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
-        <v>361</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
+      <c r="A18" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="17" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="1"/>
       <c r="C23" s="17" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2630,91 +2618,91 @@
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
-        <v>336</v>
-      </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
+      <c r="A25" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="1" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="17" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
+      <c r="A32" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="B35" s="15"/>
       <c r="C35" s="18" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2730,49 +2718,49 @@
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
-        <v>372</v>
-      </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
+      <c r="A39" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="C42" s="18"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="C43" s="1"/>
     </row>
@@ -2910,47 +2898,47 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>410</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>411</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>412</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -2975,17 +2963,17 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -3800,10 +3788,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4327,7 +4315,7 @@
         <v>129</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>130</v>
+        <v>399</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -4335,10 +4323,10 @@
         <v>48</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>132</v>
+        <v>400</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -4346,10 +4334,10 @@
         <v>49</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>134</v>
+        <v>401</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -4357,10 +4345,10 @@
         <v>50</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>136</v>
+        <v>402</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -4368,10 +4356,10 @@
         <v>51</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>138</v>
+        <v>403</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -4379,10 +4367,10 @@
         <v>52</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>140</v>
+        <v>404</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -4390,10 +4378,10 @@
         <v>53</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>142</v>
+        <v>405</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -4401,10 +4389,10 @@
         <v>54</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>144</v>
+        <v>406</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -4412,10 +4400,10 @@
         <v>55</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>146</v>
+        <v>407</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -4423,10 +4411,10 @@
         <v>56</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>148</v>
+        <v>408</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -4434,10 +4422,10 @@
         <v>57</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>150</v>
+        <v>409</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -4445,10 +4433,10 @@
         <v>58</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -4456,10 +4444,10 @@
         <v>59</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -4467,10 +4455,10 @@
         <v>60</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -4478,21 +4466,21 @@
         <v>61</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>158</v>
+        <v>410</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>62</v>
       </c>
-      <c r="B62" s="9" t="s">
-        <v>159</v>
+      <c r="B62" s="30" t="s">
+        <v>367</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>160</v>
+        <v>368</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -4500,21 +4488,21 @@
         <v>63</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>383</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>384</v>
+        <v>369</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>64</v>
       </c>
-      <c r="B64" s="30" t="s">
-        <v>385</v>
+      <c r="B64" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="C64" s="30" t="s">
-        <v>386</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -4522,21 +4510,21 @@
         <v>65</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>66</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>389</v>
+      <c r="B66" s="30" t="s">
+        <v>374</v>
       </c>
       <c r="C66" s="30" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -4544,10 +4532,10 @@
         <v>67</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="C67" s="30" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -4555,10 +4543,10 @@
         <v>68</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="C68" s="30" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -4566,10 +4554,10 @@
         <v>69</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="C69" s="30" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -4577,10 +4565,10 @@
         <v>70</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="C70" s="30" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -4588,43 +4576,10 @@
         <v>71</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="C71" s="30" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="8">
-        <v>72</v>
-      </c>
-      <c r="B72" s="30" t="s">
-        <v>400</v>
-      </c>
-      <c r="C72" s="30" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="8">
-        <v>73</v>
-      </c>
-      <c r="B73" s="30" t="s">
-        <v>402</v>
-      </c>
-      <c r="C73" s="30" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="8">
-        <v>74</v>
-      </c>
-      <c r="B74" s="30" t="s">
-        <v>403</v>
-      </c>
-      <c r="C74" s="30" t="s">
-        <v>404</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4638,7 +4593,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4655,7 +4610,7 @@
         <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4663,10 +4618,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4674,10 +4629,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4685,10 +4640,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4696,10 +4651,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>379</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -4728,19 +4683,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4748,19 +4703,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4768,17 +4723,17 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4786,13 +4741,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -4802,13 +4757,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -4818,10 +4773,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>409</v>
+        <v>388</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -4845,10 +4800,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4858,10 +4813,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4875,13 +4830,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>176</v>
+        <v>414</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4889,13 +4844,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4903,13 +4858,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4917,13 +4872,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -4931,13 +4886,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4945,13 +4900,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4959,13 +4914,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4973,13 +4928,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4987,13 +4942,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,13 +4956,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -5015,13 +4970,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5029,13 +4984,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5043,13 +4998,13 @@
         <v>13</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5057,13 +5012,27 @@
         <v>14</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>15</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -5088,775 +5057,775 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="1" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="14"/>
       <c r="C6" s="1" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
+      <c r="A8" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="15" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
+      <c r="A13" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="1" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="1"/>
       <c r="C17" s="17" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="1"/>
       <c r="C18" s="17" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
+      <c r="A20" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="1" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="17" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
+      <c r="A26" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
+      <c r="A32" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
+      <c r="A38" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="B40" s="15">
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
+      <c r="A44" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B46" s="15">
         <v>3</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="32" t="s">
-        <v>246</v>
-      </c>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
+      <c r="A50" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
+      <c r="A56" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="32" t="s">
-        <v>258</v>
-      </c>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
+      <c r="A63" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="B63" s="33"/>
+      <c r="C63" s="33"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="32" t="s">
-        <v>263</v>
-      </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="32"/>
+      <c r="A69" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32"/>
+      <c r="A74" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="B74" s="33"/>
+      <c r="C74" s="33"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32"/>
+      <c r="A79" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="B79" s="33"/>
+      <c r="C79" s="33"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B81" s="15"/>
       <c r="C81" s="1" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="17" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C83" s="21"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="B84" s="32"/>
-      <c r="C84" s="32"/>
+      <c r="A84" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="B84" s="33"/>
+      <c r="C84" s="33"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="C86" s="18" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="19" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B87" s="15"/>
       <c r="C87" s="18"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="32" t="s">
-        <v>274</v>
-      </c>
-      <c r="B90" s="32"/>
-      <c r="C90" s="32"/>
+      <c r="A90" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="B90" s="33"/>
+      <c r="C90" s="33"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="19" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C92" s="18" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="B93" s="15"/>
       <c r="C93" s="18"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="32" t="s">
-        <v>296</v>
-      </c>
-      <c r="B96" s="32"/>
-      <c r="C96" s="32"/>
+      <c r="A96" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="B96" s="33"/>
+      <c r="C96" s="33"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="16" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B98" s="15"/>
       <c r="C98" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="19" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="20" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="32" t="s">
-        <v>280</v>
-      </c>
-      <c r="B102" s="32"/>
-      <c r="C102" s="32"/>
+      <c r="A102" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="B102" s="33"/>
+      <c r="C102" s="33"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="16" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B104" s="15"/>
       <c r="C104" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="19" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="20" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="32" t="s">
-        <v>286</v>
-      </c>
-      <c r="B108" s="32"/>
-      <c r="C108" s="32"/>
+      <c r="A108" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="B108" s="33"/>
+      <c r="C108" s="33"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="19" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="19" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B111" s="15"/>
       <c r="C111" s="18" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>